<commit_message>
Changed project version in CleverCloud
</commit_message>
<xml_diff>
--- a/doc/D4/Budget.xlsx
+++ b/doc/D4/Budget.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GuilleX7\Documents\GitHub\Acme-Planner\doc\D4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263A4559-3EB3-481D-A89A-AE443222E70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C40218-E0C6-4ACE-A810-3F51FAE5CCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17970" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{E6FE04B6-807F-41B9-BCEE-B9B32721F2E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6FE04B6-807F-41B9-BCEE-B9B32721F2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$F$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$G$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -154,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -372,6 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF81983B-6797-4DAB-9661-559EA0F2B9F0}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +715,8 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -768,8 +776,8 @@
         <v>0</v>
       </c>
       <c r="G4" s="13">
-        <f>C4/3</f>
-        <v>61.111111111111114</v>
+        <f>B4-C4/3</f>
+        <v>488.88888888888891</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -796,8 +804,8 @@
         <v>0</v>
       </c>
       <c r="G5" s="13">
-        <f t="shared" ref="G5:G7" si="4">C5/3</f>
-        <v>66.666666666666671</v>
+        <f t="shared" ref="G5:G7" si="4">B5-C5/3</f>
+        <v>533.33333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -825,7 +833,7 @@
       </c>
       <c r="G6" s="13">
         <f t="shared" si="4"/>
-        <v>55.55555555555555</v>
+        <v>444.44444444444446</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -860,7 +868,7 @@
       </c>
       <c r="G7" s="13">
         <f t="shared" si="4"/>
-        <v>77.777777777777786</v>
+        <v>622.22222222222217</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -895,8 +903,8 @@
         <v>0</v>
       </c>
       <c r="G8" s="14">
-        <f>C8/3</f>
-        <v>261.11111111111114</v>
+        <f>SUM(G4:G7)</f>
+        <v>2088.8888888888887</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -915,6 +923,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="9"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -940,6 +949,7 @@
       <c r="F10" s="16" t="s">
         <v>22</v>
       </c>
+      <c r="G10" s="24"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -966,6 +976,7 @@
         <f>C11*E11</f>
         <v>25</v>
       </c>
+      <c r="G11" s="24"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -992,6 +1003,7 @@
         <f t="shared" ref="F12" si="5">C12*E12</f>
         <v>75</v>
       </c>
+      <c r="G12" s="24"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1018,6 +1030,7 @@
         <f t="shared" ref="F13" si="6">C13*E13</f>
         <v>75</v>
       </c>
+      <c r="G13" s="24"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1044,6 +1057,7 @@
         <f t="shared" ref="F14" si="7">C14*E14</f>
         <v>75</v>
       </c>
+      <c r="G14" s="24"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1070,6 +1084,7 @@
         <f t="shared" ref="F15" si="8">C15*E15</f>
         <v>75</v>
       </c>
+      <c r="G15" s="24"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1098,6 +1113,7 @@
         <f>SUM(F11:F15)</f>
         <v>325</v>
       </c>
+      <c r="G16" s="24"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1115,6 +1131,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="9"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1140,6 +1157,7 @@
       <c r="F18" s="16" t="s">
         <v>27</v>
       </c>
+      <c r="G18" s="24"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1166,6 +1184,7 @@
         <f>C19*E19</f>
         <v>8.25</v>
       </c>
+      <c r="G19" s="24"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1192,6 +1211,7 @@
         <f t="shared" ref="F20:F23" si="9">C20*E20</f>
         <v>87.5</v>
       </c>
+      <c r="G20" s="24"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1218,6 +1238,7 @@
         <f t="shared" si="9"/>
         <v>97.75</v>
       </c>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -1237,6 +1258,7 @@
         <f t="shared" si="9"/>
         <v>102</v>
       </c>
+      <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
@@ -1256,6 +1278,7 @@
         <f t="shared" si="9"/>
         <v>91.5</v>
       </c>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -1277,6 +1300,7 @@
         <f>SUM(F19:F23)</f>
         <v>387</v>
       </c>
+      <c r="G24" s="24"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
@@ -1284,7 +1308,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.31496062992125984" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>